<commit_message>
Revert "Nu minder bug"
This reverts commit b568049856747e561310f8915fdcea16feb548a0.
</commit_message>
<xml_diff>
--- a/testruns 2017-11-05.xlsx
+++ b/testruns 2017-11-05.xlsx
@@ -376,11 +376,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1801496272"/>
-        <c:axId val="-1906194320"/>
+        <c:axId val="-2027490272"/>
+        <c:axId val="-2027489728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1801496272"/>
+        <c:axId val="-2027490272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,8 +416,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.40783518345464931"/>
-              <c:y val="0.92960629921259841"/>
+              <c:x val="0.40606124234470692"/>
+              <c:y val="0.88331000291630213"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -486,7 +486,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1906194320"/>
+        <c:crossAx val="-2027489728"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -494,7 +494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1906194320"/>
+        <c:axId val="-2027489728"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -602,7 +602,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1801496272"/>
+        <c:crossAx val="-2027490272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1245,14 +1245,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>278130</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1537,10 +1537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1668,23 +1668,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>